<commit_message>
fixed nan, chart is in the excel spreadsheet.
</commit_message>
<xml_diff>
--- a/Normalized_Stats_by_DraftPos.xlsx
+++ b/Normalized_Stats_by_DraftPos.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7799A73-1E43-4406-843C-FED876EF4332}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -34,8 +40,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,7 +104,2090 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normalized PER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>13.973308275148391</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.73092452279092</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.087820832215449</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.41267992963853</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.611352026150231</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6567894721416199</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.362573585044929</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.15511205986714</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.93233384646275</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.503132652736699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.07735811258534</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.9009893942629361</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.231865239339079</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.1580919065428681</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.00630026312864</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.9109367214748332</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.2741305014040805</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.557893526503392</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.923637398973721</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.8386146118915541</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.0680577163600873</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.6696562032884881</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.8588475899206323</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.949498672454629</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.6041102131843346</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.3446015867540559</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.5967496116533315</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.5292635995011921</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.4080717488789229</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.8913293917149838</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.4630264661918577</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.3340291737539296</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.4754317336132061</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.3868958644743383</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.1123784873747233</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.9567021044322388</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.5267812655705022</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.6133140308134113</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.3004986748062421</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.4901152418149382</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.3867751529440753</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.0985421990774222</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.8515272880795077</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.2260247030131373</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.0903611553112462</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.6495584780997596</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9.0481315396113597</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.356797719609272</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.0254110612855003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.7149591813268934</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6.4476256180292051</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.6477329347284524</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7.0547725816784093</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.5588228086941598</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7.7507412580558208</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>7.6885446392172847</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.4029334828101652</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.9622374321453844</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.5498988833201439</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.9072761463908581</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9DA4-4FFA-B41D-A3E0BC734C23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normalized WS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>17.431159048609992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.76671746999429</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.304827564496071</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.60874210188944</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.74436889077773</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2602101614126298</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.3487824841415978</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.5458845956966059</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.1126412138204</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.193286201279619</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.1036813426743333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.4818468823993696</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.04706363822385</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.6075743334632389</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.0281722295785567</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.6576887661141786</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.9812062229824994</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.9536761580960462</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.3954461744516982</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5497368489958374</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.7335663547186799</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.0757420017987922</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.4599274139485416</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.9008059202189651</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.2146423612136958</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.3112338858195223</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.0719315350449561</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.5431763377186272</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.1104972375690592</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.540099236372594</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.1369028274293136</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.0555343875023819</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.7243838407585912</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.5543278084714549</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.2219585449961068</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.5564591222298096</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.2568293431553101</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.8918954191499564</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.1668601142114303</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.967652824808412</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.4028023010764938</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.8733440266143888</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.2401838808991608</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.7507996510613548</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.9172161824986631</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.6182274014578208</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.7922651933701648</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.3343183862263901</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.9418095716438248</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.7156213951794062</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.1489587760306001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.3425414364640891</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.11049723756906</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.1201883887329052</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.6273888234761351</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.4349573078854849</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.7696823204419889</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.962779877871474</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-1.624959376015599E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.5318125111388339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9DA4-4FFA-B41D-A3E0BC734C23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normalized VORP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>19.799777530589541</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.947348906192071</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.718867751125821</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.22571734093744</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.195675292449479</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.2207463630613544</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8623058542413373</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7121508811707731</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.459797785267209</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.4983821943327804</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.4820973284558256</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.337813620071683</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4644292386227891</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.3696236559139781</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0986403625699834</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.4657258064516139</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.1154001889593737</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.7328434425208634</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.4438990182328189</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.2397186974468739</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.100889419885835</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.6879833993586111</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.719665271966528</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.1889612311334714</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.7591050988553589</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.9710504549214232</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.174414927261227</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7955801104972371</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.9571203776553889</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.8524758578179572</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.0004743833017069</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.6070634037819782</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.65560454861916906</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.88777446462455922</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.2054557263476946</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.9391083725987679</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.443717572749831</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.349504699009398</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.2672811059907829</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.70889698231009368</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.360551075268817</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.78910856746444669</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.536321103176558</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.18675721561969449</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.7828481510621552</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.0449986446191373</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.4774193548387089</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.5045011252813199</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.230899830220713</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.76214108472172981</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.6054590570719589</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.2450076804915522</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-0.27763088313061868</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.665785298783713</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.4926686217008802</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.93245967741935476</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.84889643463497455</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-0.99620493358633788</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.9947970863683668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9DA4-4FFA-B41D-A3E0BC734C23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="502177688"/>
+        <c:axId val="502178016"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="502177688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="502178016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="502178016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="502177688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7171242-E271-49C9-8BAE-DE95A11D1476}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -144,7 +2233,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +2265,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +2317,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,14 +2510,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +2536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -420,16 +2547,16 @@
         <v>43</v>
       </c>
       <c r="D2">
-        <v>13.97330827514839</v>
+        <v>13.973308275148391</v>
       </c>
       <c r="E2">
-        <v>17.43115904860999</v>
+        <v>17.431159048609992</v>
       </c>
       <c r="F2">
-        <v>19.79977753058954</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>19.799777530589541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -446,10 +2573,10 @@
         <v>12.76671746999429</v>
       </c>
       <c r="F3">
-        <v>10.94734890619207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>10.947348906192071</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -460,16 +2587,16 @@
         <v>43</v>
       </c>
       <c r="D4">
-        <v>12.08782083221545</v>
+        <v>12.087820832215449</v>
       </c>
       <c r="E4">
-        <v>14.30482756449607</v>
+        <v>14.304827564496071</v>
       </c>
       <c r="F4">
-        <v>13.71886775112582</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>13.718867751125821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -489,7 +2616,7 @@
         <v>11.22571734093744</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -500,16 +2627,16 @@
         <v>43</v>
       </c>
       <c r="D6">
-        <v>11.61135202615023</v>
+        <v>11.611352026150231</v>
       </c>
       <c r="E6">
         <v>12.74436889077773</v>
       </c>
       <c r="F6">
-        <v>13.19567529244948</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>13.195675292449479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -520,16 +2647,16 @@
         <v>43</v>
       </c>
       <c r="D7">
-        <v>9.65678947214162</v>
+        <v>9.6567894721416199</v>
       </c>
       <c r="E7">
-        <v>8.26021016141263</v>
+        <v>8.2602101614126298</v>
       </c>
       <c r="F7">
-        <v>6.220746363061354</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>6.2207463630613544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -540,16 +2667,16 @@
         <v>43</v>
       </c>
       <c r="D8">
-        <v>10.36257358504493</v>
+        <v>10.362573585044929</v>
       </c>
       <c r="E8">
-        <v>9.348782484141598</v>
+        <v>9.3487824841415978</v>
       </c>
       <c r="F8">
-        <v>6.862305854241337</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>6.8623058542413373</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -563,13 +2690,13 @@
         <v>10.15511205986714</v>
       </c>
       <c r="E9">
-        <v>8.545884595696606</v>
+        <v>8.5458845956966059</v>
       </c>
       <c r="F9">
-        <v>5.712150881170773</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>5.7121508811707731</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -586,10 +2713,10 @@
         <v>12.1126412138204</v>
       </c>
       <c r="F10">
-        <v>10.45979778526721</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>10.459797785267209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -600,16 +2727,16 @@
         <v>43</v>
       </c>
       <c r="D11">
-        <v>10.5031326527367</v>
+        <v>10.503132652736699</v>
       </c>
       <c r="E11">
-        <v>10.19328620127962</v>
+        <v>10.193286201279619</v>
       </c>
       <c r="F11">
-        <v>8.49838219433278</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>8.4983821943327804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -623,13 +2750,13 @@
         <v>10.07735811258534</v>
       </c>
       <c r="E12">
-        <v>9.103681342674333</v>
+        <v>9.1036813426743333</v>
       </c>
       <c r="F12">
-        <v>6.482097328455826</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>6.4820973284558256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -640,16 +2767,16 @@
         <v>43</v>
       </c>
       <c r="D13">
-        <v>8.900989394262936</v>
+        <v>8.9009893942629361</v>
       </c>
       <c r="E13">
-        <v>6.48184688239937</v>
+        <v>6.4818468823993696</v>
       </c>
       <c r="F13">
         <v>3.337813620071683</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -660,16 +2787,16 @@
         <v>43</v>
       </c>
       <c r="D14">
-        <v>10.23186523933908</v>
+        <v>10.231865239339079</v>
       </c>
       <c r="E14">
         <v>10.04706363822385</v>
       </c>
       <c r="F14">
-        <v>7.464429238622789</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>7.4644292386227891</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -680,13 +2807,16 @@
         <v>43</v>
       </c>
       <c r="D15">
-        <v>9.158091906542868</v>
+        <v>9.1580919065428681</v>
       </c>
       <c r="E15">
-        <v>7.607574333463239</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>7.6075743334632389</v>
+      </c>
+      <c r="F15">
+        <v>5.3696236559139781</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -700,13 +2830,13 @@
         <v>10.00630026312864</v>
       </c>
       <c r="E16">
-        <v>8.028172229578557</v>
+        <v>8.0281722295785567</v>
       </c>
       <c r="F16">
-        <v>5.098640362569983</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>5.0986403625699834</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -717,16 +2847,16 @@
         <v>43</v>
       </c>
       <c r="D17">
-        <v>9.910936721474833</v>
+        <v>9.9109367214748332</v>
       </c>
       <c r="E17">
-        <v>7.657688766114179</v>
+        <v>7.6576887661141786</v>
       </c>
       <c r="F17">
-        <v>4.465725806451614</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>4.4657258064516139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -737,16 +2867,16 @@
         <v>42</v>
       </c>
       <c r="D18">
-        <v>9.27413050140408</v>
+        <v>9.2741305014040805</v>
       </c>
       <c r="E18">
-        <v>6.981206222982499</v>
+        <v>6.9812062229824994</v>
       </c>
       <c r="F18">
-        <v>5.115400188959374</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>5.1154001889593737</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -760,10 +2890,13 @@
         <v>9.557893526503392</v>
       </c>
       <c r="E19">
-        <v>7.953676158096046</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>7.9536761580960462</v>
+      </c>
+      <c r="F19">
+        <v>4.7328434425208634</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -777,10 +2910,13 @@
         <v>8.923637398973721</v>
       </c>
       <c r="E20">
-        <v>6.395446174451698</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>6.3954461744516982</v>
+      </c>
+      <c r="F20">
+        <v>2.4438990182328189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -791,16 +2927,16 @@
         <v>42</v>
       </c>
       <c r="D21">
-        <v>8.838614611891554</v>
+        <v>8.8386146118915541</v>
       </c>
       <c r="E21">
-        <v>5.549736848995837</v>
+        <v>5.5497368489958374</v>
       </c>
       <c r="F21">
-        <v>2.239718697446874</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>2.2397186974468739</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -811,13 +2947,16 @@
         <v>43</v>
       </c>
       <c r="D22">
-        <v>9.068057716360087</v>
+        <v>9.0680577163600873</v>
       </c>
       <c r="E22">
-        <v>6.73356635471868</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>6.7335663547186799</v>
+      </c>
+      <c r="F22">
+        <v>5.100889419885835</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -828,13 +2967,16 @@
         <v>43</v>
       </c>
       <c r="D23">
-        <v>8.669656203288488</v>
+        <v>8.6696562032884881</v>
       </c>
       <c r="E23">
-        <v>6.075742001798792</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>6.0757420017987922</v>
+      </c>
+      <c r="F23">
+        <v>3.6879833993586111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -845,16 +2987,16 @@
         <v>41</v>
       </c>
       <c r="D24">
-        <v>8.858847589920632</v>
+        <v>8.8588475899206323</v>
       </c>
       <c r="E24">
-        <v>6.459927413948542</v>
+        <v>6.4599274139485416</v>
       </c>
       <c r="F24">
         <v>2.719665271966528</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -867,8 +3009,14 @@
       <c r="D25">
         <v>8.949498672454629</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="E25">
+        <v>7.9008059202189651</v>
+      </c>
+      <c r="F25">
+        <v>6.1889612311334714</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -879,13 +3027,16 @@
         <v>42</v>
       </c>
       <c r="D26">
-        <v>8.604110213184335</v>
+        <v>8.6041102131843346</v>
       </c>
       <c r="E26">
-        <v>5.214642361213696</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>5.2146423612136958</v>
+      </c>
+      <c r="F26">
+        <v>3.7591050988553589</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -896,16 +3047,16 @@
         <v>40</v>
       </c>
       <c r="D27">
-        <v>9.344601586754056</v>
+        <v>9.3446015867540559</v>
       </c>
       <c r="E27">
-        <v>7.311233885819522</v>
+        <v>7.3112338858195223</v>
       </c>
       <c r="F27">
-        <v>4.971050454921423</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>4.9710504549214232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -916,16 +3067,16 @@
         <v>42</v>
       </c>
       <c r="D28">
-        <v>8.596749611653332</v>
+        <v>8.5967496116533315</v>
       </c>
       <c r="E28">
-        <v>6.071931535044956</v>
+        <v>6.0719315350449561</v>
       </c>
       <c r="F28">
         <v>3.174414927261227</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -936,16 +3087,16 @@
         <v>40</v>
       </c>
       <c r="D29">
-        <v>8.529263599501192</v>
+        <v>8.5292635995011921</v>
       </c>
       <c r="E29">
-        <v>5.543176337718627</v>
+        <v>5.5431763377186272</v>
       </c>
       <c r="F29">
-        <v>1.795580110497237</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>1.7955801104972371</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -956,16 +3107,16 @@
         <v>37</v>
       </c>
       <c r="D30">
-        <v>8.408071748878923</v>
+        <v>8.4080717488789229</v>
       </c>
       <c r="E30">
-        <v>5.110497237569059</v>
+        <v>5.1104972375690592</v>
       </c>
       <c r="F30">
-        <v>1.957120377655389</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>1.9571203776553889</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -976,16 +3127,16 @@
         <v>40</v>
       </c>
       <c r="D31">
-        <v>7.891329391714984</v>
+        <v>7.8913293917149838</v>
       </c>
       <c r="E31">
         <v>6.540099236372594</v>
       </c>
       <c r="F31">
-        <v>3.852475857817957</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>3.8524758578179572</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -996,16 +3147,16 @@
         <v>39</v>
       </c>
       <c r="D32">
-        <v>8.463026466191858</v>
+        <v>8.4630264661918577</v>
       </c>
       <c r="E32">
-        <v>5.136902827429314</v>
+        <v>5.1369028274293136</v>
       </c>
       <c r="F32">
-        <v>3.000474383301707</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>3.0004743833017069</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1016,16 +3167,16 @@
         <v>38</v>
       </c>
       <c r="D33">
-        <v>7.33402917375393</v>
+        <v>7.3340291737539296</v>
       </c>
       <c r="E33">
-        <v>4.055534387502382</v>
+        <v>4.0555343875023819</v>
       </c>
       <c r="F33">
-        <v>2.607063403781978</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>2.6070634037819782</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1036,13 +3187,16 @@
         <v>41</v>
       </c>
       <c r="D34">
-        <v>7.475431733613206</v>
+        <v>7.4754317336132061</v>
       </c>
       <c r="E34">
-        <v>3.724383840758591</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>3.7243838407585912</v>
+      </c>
+      <c r="F34">
+        <v>0.65560454861916906</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1053,13 +3207,16 @@
         <v>38</v>
       </c>
       <c r="D35">
-        <v>8.386895864474338</v>
+        <v>8.3868958644743383</v>
       </c>
       <c r="E35">
-        <v>3.554327808471455</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>3.5543278084714549</v>
+      </c>
+      <c r="F35">
+        <v>0.88777446462455922</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1070,16 +3227,16 @@
         <v>39</v>
       </c>
       <c r="D36">
-        <v>8.112378487374723</v>
+        <v>8.1123784873747233</v>
       </c>
       <c r="E36">
-        <v>6.221958544996107</v>
+        <v>6.2219585449961068</v>
       </c>
       <c r="F36">
-        <v>4.205455726347695</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>4.2054557263476946</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1090,16 +3247,16 @@
         <v>36</v>
       </c>
       <c r="D37">
-        <v>7.956702104432239</v>
+        <v>7.9567021044322388</v>
       </c>
       <c r="E37">
-        <v>4.55645912222981</v>
+        <v>4.5564591222298096</v>
       </c>
       <c r="F37">
-        <v>1.939108372598768</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>1.9391083725987679</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1110,13 +3267,16 @@
         <v>38</v>
       </c>
       <c r="D38">
-        <v>7.526781265570502</v>
+        <v>7.5267812655705022</v>
       </c>
       <c r="E38">
-        <v>4.25682934315531</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>4.2568293431553101</v>
+      </c>
+      <c r="F38">
+        <v>1.443717572749831</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1127,16 +3287,16 @@
         <v>34</v>
       </c>
       <c r="D39">
-        <v>7.613314030813411</v>
+        <v>7.6133140308134113</v>
       </c>
       <c r="E39">
-        <v>4.891895419149956</v>
+        <v>4.8918954191499564</v>
       </c>
       <c r="F39">
         <v>2.349504699009398</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1147,16 +3307,16 @@
         <v>33</v>
       </c>
       <c r="D40">
-        <v>7.300498674806242</v>
+        <v>7.3004986748062421</v>
       </c>
       <c r="E40">
-        <v>4.16686011421143</v>
+        <v>4.1668601142114303</v>
       </c>
       <c r="F40">
-        <v>1.267281105990783</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>1.2672811059907829</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1167,16 +3327,16 @@
         <v>35</v>
       </c>
       <c r="D41">
-        <v>7.490115241814938</v>
+        <v>7.4901152418149382</v>
       </c>
       <c r="E41">
         <v>3.967652824808412</v>
       </c>
       <c r="F41">
-        <v>0.7088969823100937</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>0.70889698231009368</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1187,13 +3347,16 @@
         <v>35</v>
       </c>
       <c r="D42">
-        <v>7.386775152944075</v>
+        <v>7.3867751529440753</v>
       </c>
       <c r="E42">
-        <v>4.402802301076494</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>4.4028023010764938</v>
+      </c>
+      <c r="F42">
+        <v>2.360551075268817</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1204,16 +3367,16 @@
         <v>29</v>
       </c>
       <c r="D43">
-        <v>7.098542199077422</v>
+        <v>7.0985421990774222</v>
       </c>
       <c r="E43">
-        <v>3.873344026614389</v>
+        <v>3.8733440266143888</v>
       </c>
       <c r="F43">
-        <v>0.7891085674644467</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>0.78910856746444669</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1224,16 +3387,16 @@
         <v>35</v>
       </c>
       <c r="D44">
-        <v>7.851527288079508</v>
+        <v>7.8515272880795077</v>
       </c>
       <c r="E44">
-        <v>5.240183880899161</v>
+        <v>5.2401838808991608</v>
       </c>
       <c r="F44">
         <v>2.536321103176558</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1244,16 +3407,16 @@
         <v>26</v>
       </c>
       <c r="D45">
-        <v>7.226024703013137</v>
+        <v>7.2260247030131373</v>
       </c>
       <c r="E45">
-        <v>2.750799651061355</v>
+        <v>2.7507996510613548</v>
       </c>
       <c r="F45">
-        <v>0.1867572156196945</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>0.18675721561969449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1264,13 +3427,16 @@
         <v>35</v>
       </c>
       <c r="D46">
-        <v>9.090361155311246</v>
+        <v>9.0903611553112462</v>
       </c>
       <c r="E46">
-        <v>6.917216182498663</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>6.9172161824986631</v>
+      </c>
+      <c r="F46">
+        <v>5.7828481510621552</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1281,13 +3447,16 @@
         <v>33</v>
       </c>
       <c r="D47">
-        <v>8.64955847809976</v>
+        <v>8.6495584780997596</v>
       </c>
       <c r="E47">
-        <v>6.618227401457821</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>6.6182274014578208</v>
+      </c>
+      <c r="F47">
+        <v>6.0449986446191373</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1298,16 +3467,16 @@
         <v>31</v>
       </c>
       <c r="D48">
-        <v>9.04813153961136</v>
+        <v>9.0481315396113597</v>
       </c>
       <c r="E48">
-        <v>5.792265193370165</v>
+        <v>5.7922651933701648</v>
       </c>
       <c r="F48">
-        <v>3.477419354838709</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>3.4774193548387089</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1321,13 +3490,13 @@
         <v>8.356797719609272</v>
       </c>
       <c r="E49">
-        <v>6.33431838622639</v>
+        <v>6.3343183862263901</v>
       </c>
       <c r="F49">
-        <v>5.50450112528132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>5.5045011252813199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1338,13 +3507,16 @@
         <v>28</v>
       </c>
       <c r="D50">
-        <v>7.0254110612855</v>
+        <v>7.0254110612855003</v>
       </c>
       <c r="E50">
-        <v>2.941809571643825</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>2.9418095716438248</v>
+      </c>
+      <c r="F50">
+        <v>1.230899830220713</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1355,16 +3527,16 @@
         <v>33</v>
       </c>
       <c r="D51">
-        <v>6.714959181326893</v>
+        <v>6.7149591813268934</v>
       </c>
       <c r="E51">
-        <v>3.715621395179406</v>
+        <v>3.7156213951794062</v>
       </c>
       <c r="F51">
-        <v>0.7621410847217298</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>0.76214108472172981</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1375,16 +3547,16 @@
         <v>24</v>
       </c>
       <c r="D52">
-        <v>6.447625618029205</v>
+        <v>6.4476256180292051</v>
       </c>
       <c r="E52">
-        <v>4.1489587760306</v>
+        <v>4.1489587760306001</v>
       </c>
       <c r="F52">
-        <v>2.605459057071959</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>2.6054590570719589</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1395,16 +3567,16 @@
         <v>29</v>
       </c>
       <c r="D53">
-        <v>6.647732934728452</v>
+        <v>6.6477329347284524</v>
       </c>
       <c r="E53">
-        <v>2.342541436464089</v>
+        <v>2.3425414364640891</v>
       </c>
       <c r="F53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1415,16 +3587,16 @@
         <v>29</v>
       </c>
       <c r="D54">
-        <v>7.054772581678409</v>
+        <v>7.0547725816784093</v>
       </c>
       <c r="E54">
         <v>5.11049723756906</v>
       </c>
       <c r="F54">
-        <v>3.245007680491552</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>3.2450076804915522</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1435,16 +3607,16 @@
         <v>26</v>
       </c>
       <c r="D55">
-        <v>5.55882280869416</v>
+        <v>5.5588228086941598</v>
       </c>
       <c r="E55">
-        <v>3.120188388732905</v>
+        <v>3.1201883887329052</v>
       </c>
       <c r="F55">
-        <v>-0.2776308831306187</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>-0.27763088313061868</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1455,16 +3627,16 @@
         <v>21</v>
       </c>
       <c r="D56">
-        <v>7.750741258055821</v>
+        <v>7.7507412580558208</v>
       </c>
       <c r="E56">
-        <v>3.627388823476135</v>
+        <v>3.6273888234761351</v>
       </c>
       <c r="F56">
         <v>1.665785298783713</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1475,16 +3647,16 @@
         <v>23</v>
       </c>
       <c r="D57">
-        <v>7.688544639217285</v>
+        <v>7.6885446392172847</v>
       </c>
       <c r="E57">
-        <v>4.434957307885485</v>
+        <v>4.4349573078854849</v>
       </c>
       <c r="F57">
-        <v>2.49266862170088</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>2.4926686217008802</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1495,16 +3667,16 @@
         <v>23</v>
       </c>
       <c r="D58">
-        <v>3.402933482810165</v>
+        <v>3.4029334828101652</v>
       </c>
       <c r="E58">
-        <v>1.769682320441989</v>
+        <v>1.7696823204419889</v>
       </c>
       <c r="F58">
-        <v>0.9324596774193548</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>0.93245967741935476</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1515,16 +3687,16 @@
         <v>22</v>
       </c>
       <c r="D59">
-        <v>4.962237432145384</v>
+        <v>4.9622374321453844</v>
       </c>
       <c r="E59">
         <v>1.962779877871474</v>
       </c>
       <c r="F59">
-        <v>0.8488964346349746</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>0.84889643463497455</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1535,16 +3707,16 @@
         <v>16</v>
       </c>
       <c r="D60">
-        <v>2.549898883320144</v>
+        <v>2.5498988833201439</v>
       </c>
       <c r="E60">
-        <v>-0.01624959376015599</v>
+        <v>-1.624959376015599E-2</v>
       </c>
       <c r="F60">
-        <v>-0.9962049335863379</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>-0.99620493358633788</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1555,16 +3727,17 @@
         <v>18</v>
       </c>
       <c r="D61">
-        <v>6.907276146390858</v>
+        <v>6.9072761463908581</v>
       </c>
       <c r="E61">
-        <v>6.531812511138834</v>
+        <v>6.5318125111388339</v>
       </c>
       <c r="F61">
-        <v>4.994797086368367</v>
+        <v>4.9947970863683668</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>